<commit_message>
Add phase into API
</commit_message>
<xml_diff>
--- a/data/api.xlsx
+++ b/data/api.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/excelcy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FECDF8-C395-7545-8E4D-E9B69D95BC24}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2AD9EF-122B-8E46-8E2B-D82A034BBBEA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="source" sheetId="4" r:id="rId1"/>
-    <sheet name="prepare" sheetId="3" r:id="rId2"/>
-    <sheet name="train" sheetId="1" r:id="rId3"/>
-    <sheet name="config" sheetId="2" r:id="rId4"/>
+    <sheet name="phase" sheetId="5" r:id="rId1"/>
+    <sheet name="source" sheetId="4" r:id="rId2"/>
+    <sheet name="prepare" sheetId="3" r:id="rId3"/>
+    <sheet name="train" sheetId="1" r:id="rId4"/>
+    <sheet name="config" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t>text</t>
   </si>
@@ -152,6 +153,45 @@
   </si>
   <si>
     <t>source/source_01.txt</t>
+  </si>
+  <si>
+    <t>discover</t>
+  </si>
+  <si>
+    <t>prepare</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>fn</t>
+  </si>
+  <si>
+    <t>export_entity</t>
+  </si>
+  <si>
+    <t>save_nlp</t>
+  </si>
+  <si>
+    <t>save_storage</t>
+  </si>
+  <si>
+    <t>file_path=nlp/data-[date]</t>
+  </si>
+  <si>
+    <t>args</t>
+  </si>
+  <si>
+    <t>file_path=nlp/data</t>
+  </si>
+  <si>
+    <t>file_path=[storage-name].xlsx</t>
+  </si>
+  <si>
+    <t>file_path=person.xlsx, label=PERSON</t>
   </si>
 </sst>
 </file>
@@ -493,48 +533,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BF5D81-E310-3A45-9ABE-A86114765ABD}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BBB3E5-6C1D-7646-B12D-3BE01DC03441}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
-    <col min="3" max="3" width="78.5" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="B2" t="b">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>30</v>
+      <c r="B3" t="b">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -544,6 +650,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BF5D81-E310-3A45-9ABE-A86114765ABD}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="78.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B93662-D338-7A4C-897B-C0C87D585A42}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -603,7 +772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -744,7 +913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fix overlap token during NER training, add poetry and update documentation
</commit_message>
<xml_diff>
--- a/data/api.xlsx
+++ b/data/api.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/excelcy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/kororo/excelcy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2AD9EF-122B-8E46-8E2B-D82A034BBBEA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA2432A-AF12-D34C-9545-22D55E072C61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>